<commit_message>
fix: add dj-database-url for DB settings and several samples for site
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Реверсивный инжениринг</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Кабель</t>
+  </si>
+  <si>
+    <t>Шестерня планетарная</t>
+  </si>
+  <si>
+    <t>planetary gear 2.jpg</t>
+  </si>
+  <si>
+    <t>planetary gear 1.jpg</t>
   </si>
 </sst>
 </file>
@@ -397,10 +406,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -551,6 +560,28 @@
       </c>
       <c r="C13" s="3" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>